<commit_message>
Se agrego cambios en las alertas de la subida de archivos y además se agregó el boto descargar plantilla
</commit_message>
<xml_diff>
--- a/schedule-management-backend/src/main/resources/files/templates/Plantilla_oferta_academica.xlsx
+++ b/schedule-management-backend/src/main/resources/files/templates/Plantilla_oferta_academica.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNIVERSIDAD\OCTAVO SEMESTRE\Proyecto_1\project-1-folder\schedule-management-unicauca\schedule-management-backend\src\main\resources\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E64BFC-CD39-4138-AB9A-3041428FDD36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FE139B-844E-4F26-B1EB-B28E50A8BB81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{BB4D6D1C-47BE-482B-8849-6E1103E0D03C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{BB4D6D1C-47BE-482B-8849-6E1103E0D03C}"/>
   </bookViews>
   <sheets>
     <sheet name="OFERTA ACADÉMICA" sheetId="1" r:id="rId1"/>
@@ -1991,7 +1991,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{671A567B-3082-469A-8251-59A6BD077B24}">
   <dimension ref="A1:AD26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -2840,10 +2840,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50281456-BAF9-43C0-BD22-EAB2E8D38C04}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2973,6 +2973,56 @@
       <c r="A23" s="14"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="14"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="14"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="14"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cambio del formato de plantilla oferta academica
</commit_message>
<xml_diff>
--- a/schedule-management-backend/src/main/resources/files/templates/Plantilla_oferta_academica.xlsx
+++ b/schedule-management-backend/src/main/resources/files/templates/Plantilla_oferta_academica.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNIVERSIDAD\OCTAVO SEMESTRE\Proyecto_1\project-1-folder\schedule-management-unicauca\schedule-management-backend\src\main\resources\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FE139B-844E-4F26-B1EB-B28E50A8BB81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E13ED3-FCC8-461C-8E52-330617338B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{BB4D6D1C-47BE-482B-8849-6E1103E0D03C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{BB4D6D1C-47BE-482B-8849-6E1103E0D03C}"/>
   </bookViews>
   <sheets>
     <sheet name="OFERTA ACADÉMICA" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="60">
   <si>
     <t>INFORMACION DEL PROGRAMA</t>
   </si>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t>PROFESOR 3</t>
-  </si>
-  <si>
-    <t>INTRO1 - Introducción a la programación</t>
   </si>
   <si>
     <t>Erwin Meza Vega</t>
@@ -818,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C001AD1-C0D2-4B06-86EF-ABBCED52D1B0}">
   <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,30 +925,32 @@
         <v>1</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="8">
+        <v>59</v>
+      </c>
+      <c r="C11" s="8" t="e">
         <f>+VLOOKUP(B11,'MATERIAS 3'!D$1:F$11,2,FALSE)</f>
-        <v>2</v>
-      </c>
-      <c r="D11" s="8">
+        <v>#N/A</v>
+      </c>
+      <c r="D11" s="8" t="e">
         <f>+VLOOKUP(B11,'MATERIAS 3'!D$1:F$11,3,FALSE)</f>
-        <v>4</v>
+        <v>#N/A</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
+      <c r="A12" s="8">
+        <v>2</v>
+      </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -962,7 +961,9 @@
       <c r="I12" s="8"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
+      <c r="A13" s="8">
+        <v>3</v>
+      </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -1935,7 +1936,7 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A4:B4"/>
   </mergeCells>
-  <dataValidations count="8">
+  <dataValidations count="9">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="FECHA DE FINALIZACION NO VALIDA" error="La fecha de finalizacion debe ser mayor que la fecha inicial" sqref="B7" xr:uid="{8DDE76B2-4CBC-40C5-9E1F-9D24A6784581}">
       <formula1>B6</formula1>
     </dataValidation>
@@ -1945,9 +1946,6 @@
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="PERIODO NO VALIDO" error="El periodo debe 1 o 2" sqref="B5" xr:uid="{6DAB2920-DB78-4AED-8ECD-11147274C444}">
       <formula1>1</formula1>
       <formula2>2</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24:B100" xr:uid="{FED918D0-4941-4519-96E8-A8311C2B00B4}">
-      <formula1>INDIRECT(CONCATENATE("semestre_",A24))</formula1>
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11:D100" xr:uid="{F1960164-EFB6-4858-9B12-63DCD65486C8}">
       <formula1>2</formula1>
@@ -1961,25 +1959,25 @@
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{3FA7B6A6-08C5-4352-A47D-37F7C0185C70}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B48:B100" xr:uid="{3FA7B6A6-08C5-4352-A47D-37F7C0185C70}">
       <formula1>INDIRECT(CONCATENATE("semestre_",$A$11:$A$30))</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16:B47" xr:uid="{37C94168-E69D-45C5-A4E7-940C8421B061}">
+      <formula1>INDIRECT(CONCATENATE("semestre_",$A$12))</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:B15" xr:uid="{64576F12-3A2E-4378-AB12-0342EB0C8F2F}">
+      <formula1>INDIRECT(CONCATENATE("semestre_",$A11))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{63422297-7960-4B02-93AB-1B26DEC09764}">
           <x14:formula1>
             <xm:f>DOCENTES!$B$2:$B$400</xm:f>
           </x14:formula1>
           <xm:sqref>G11:I100</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{53F5ED31-2A8C-42F8-A4C9-BF133E68930E}">
-          <x14:formula1>
-            <xm:f>'MATERIAS 3'!$D$2:$D$11</xm:f>
-          </x14:formula1>
-          <xm:sqref>B12:B23</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2022,7 +2020,7 @@
   <sheetData>
     <row r="1" spans="1:30" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -2056,52 +2054,52 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="25"/>
       <c r="C2" s="26"/>
       <c r="D2" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E2" s="25"/>
       <c r="F2" s="26"/>
       <c r="G2" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H2" s="25"/>
       <c r="I2" s="26"/>
       <c r="J2" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K2" s="25"/>
       <c r="L2" s="26"/>
       <c r="M2" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N2" s="25"/>
       <c r="O2" s="26"/>
       <c r="P2" s="24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q2" s="25"/>
       <c r="R2" s="26"/>
       <c r="S2" s="24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="T2" s="25"/>
       <c r="U2" s="26"/>
       <c r="V2" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="W2" s="25"/>
       <c r="X2" s="26"/>
       <c r="Y2" s="24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Z2" s="25"/>
       <c r="AA2" s="26"/>
       <c r="AB2" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC2" s="25"/>
       <c r="AD2" s="26"/>
@@ -2111,7 +2109,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>13</v>
@@ -2120,7 +2118,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>13</v>
@@ -2129,7 +2127,7 @@
         <v>11</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>13</v>
@@ -2138,7 +2136,7 @@
         <v>11</v>
       </c>
       <c r="K3" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>13</v>
@@ -2147,7 +2145,7 @@
         <v>11</v>
       </c>
       <c r="N3" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O3" s="7" t="s">
         <v>13</v>
@@ -2156,7 +2154,7 @@
         <v>11</v>
       </c>
       <c r="Q3" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R3" s="7" t="s">
         <v>13</v>
@@ -2165,7 +2163,7 @@
         <v>11</v>
       </c>
       <c r="T3" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="U3" s="7" t="s">
         <v>13</v>
@@ -2174,7 +2172,7 @@
         <v>11</v>
       </c>
       <c r="W3" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="X3" s="7" t="s">
         <v>13</v>
@@ -2183,7 +2181,7 @@
         <v>11</v>
       </c>
       <c r="Z3" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AA3" s="7" t="s">
         <v>13</v>
@@ -2192,7 +2190,7 @@
         <v>11</v>
       </c>
       <c r="AC3" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AD3" s="7" t="s">
         <v>13</v>
@@ -2200,91 +2198,91 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="8">
         <v>4</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F4" s="8">
         <v>4</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I4" s="8">
         <v>4</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K4" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L4" s="8">
         <v>4</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N4" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O4" s="8">
         <v>4</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q4" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R4" s="8">
         <v>4</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="T4" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U4" s="8">
         <v>4</v>
       </c>
       <c r="V4" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="W4" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="X4" s="8">
         <v>4</v>
       </c>
       <c r="Y4" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Z4" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AA4" s="8">
         <v>4</v>
       </c>
       <c r="AB4" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AC4" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AD4" s="8">
         <v>4</v>
@@ -2842,7 +2840,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50281456-BAF9-43C0-BD22-EAB2E8D38C04}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
@@ -2855,13 +2853,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3052,16 +3050,16 @@
         <v>10</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>11</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>13</v>
@@ -3072,10 +3070,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>24</v>
       </c>
       <c r="D2" s="8" t="str">
         <f>CONCATENATE(B2," - ",C2)</f>
@@ -3093,10 +3091,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="D3" s="8" t="str">
         <f>CONCATENATE(B3," - ",C3)</f>
@@ -3114,10 +3112,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D4" s="8" t="str">
         <f t="shared" ref="D4:D11" si="0">CONCATENATE(B4," - ",C4)</f>
@@ -3135,10 +3133,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>30</v>
       </c>
       <c r="D5" s="8" t="str">
         <f>CONCATENATE(B5," - ",C5)</f>
@@ -3156,10 +3154,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>32</v>
       </c>
       <c r="D6" s="8" t="str">
         <f t="shared" si="0"/>
@@ -3177,10 +3175,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>34</v>
       </c>
       <c r="D7" s="8" t="str">
         <f>CONCATENATE(B7," - ",C7)</f>
@@ -3198,10 +3196,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>36</v>
       </c>
       <c r="D8" s="8" t="str">
         <f t="shared" si="0"/>
@@ -3219,10 +3217,10 @@
         <v>4</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="D9" s="8" t="str">
         <f t="shared" si="0"/>
@@ -3240,10 +3238,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="D10" s="8" t="str">
         <f t="shared" si="0"/>
@@ -3261,10 +3259,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>42</v>
       </c>
       <c r="D11" s="8" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Servicio de descarga de Plantilla_Ambientes con correcciones generales
</commit_message>
<xml_diff>
--- a/schedule-management-backend/src/main/resources/files/templates/Plantilla_oferta_academica.xlsx
+++ b/schedule-management-backend/src/main/resources/files/templates/Plantilla_oferta_academica.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNIVERSIDAD\OCTAVO SEMESTRE\Proyecto_1\project-1-folder\schedule-management-unicauca\schedule-management-backend\src\main\resources\files\templates\"/>
     </mc:Choice>
@@ -32,7 +32,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -237,6 +237,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -821,15 +822,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="39" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="27.5703125" customWidth="1"/>
-    <col min="8" max="8" width="28" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="22.7109375"/>
+    <col min="2" max="2" customWidth="true" width="39.0"/>
+    <col min="3" max="3" customWidth="true" width="21.42578125"/>
+    <col min="4" max="4" customWidth="true" width="23.5703125"/>
+    <col min="5" max="5" customWidth="true" width="10.85546875"/>
+    <col min="6" max="6" customWidth="true" width="11.28515625"/>
+    <col min="7" max="7" customWidth="true" width="27.5703125"/>
+    <col min="8" max="8" customWidth="true" width="28.0"/>
+    <col min="9" max="9" customWidth="true" width="22.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1995,27 +1996,27 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
-    <col min="4" max="4" width="23" style="18" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" customWidth="1"/>
-    <col min="7" max="8" width="22.7109375" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" customWidth="1"/>
-    <col min="10" max="11" width="22.7109375" customWidth="1"/>
-    <col min="12" max="12" width="21.5703125" customWidth="1"/>
-    <col min="13" max="14" width="22.7109375" customWidth="1"/>
-    <col min="15" max="15" width="21.5703125" customWidth="1"/>
-    <col min="16" max="17" width="22.7109375" customWidth="1"/>
-    <col min="18" max="18" width="21.5703125" customWidth="1"/>
-    <col min="19" max="20" width="22.7109375" customWidth="1"/>
-    <col min="21" max="21" width="21.5703125" customWidth="1"/>
-    <col min="22" max="23" width="22.7109375" customWidth="1"/>
-    <col min="24" max="24" width="21.5703125" customWidth="1"/>
-    <col min="25" max="26" width="22.7109375" customWidth="1"/>
-    <col min="27" max="27" width="21.5703125" customWidth="1"/>
-    <col min="28" max="29" width="22.7109375" customWidth="1"/>
-    <col min="30" max="30" width="21.5703125" customWidth="1"/>
+    <col min="1" max="2" customWidth="true" width="22.7109375"/>
+    <col min="3" max="3" customWidth="true" width="21.5703125"/>
+    <col min="4" max="4" customWidth="true" style="18" width="23.0"/>
+    <col min="5" max="5" customWidth="true" width="20.7109375"/>
+    <col min="6" max="6" customWidth="true" width="25.5703125"/>
+    <col min="7" max="8" customWidth="true" width="22.7109375"/>
+    <col min="9" max="9" customWidth="true" width="21.5703125"/>
+    <col min="10" max="11" customWidth="true" width="22.7109375"/>
+    <col min="12" max="12" customWidth="true" width="21.5703125"/>
+    <col min="13" max="14" customWidth="true" width="22.7109375"/>
+    <col min="15" max="15" customWidth="true" width="21.5703125"/>
+    <col min="16" max="17" customWidth="true" width="22.7109375"/>
+    <col min="18" max="18" customWidth="true" width="21.5703125"/>
+    <col min="19" max="20" customWidth="true" width="22.7109375"/>
+    <col min="21" max="21" customWidth="true" width="21.5703125"/>
+    <col min="22" max="23" customWidth="true" width="22.7109375"/>
+    <col min="24" max="24" customWidth="true" width="21.5703125"/>
+    <col min="25" max="26" customWidth="true" width="22.7109375"/>
+    <col min="27" max="27" customWidth="true" width="21.5703125"/>
+    <col min="28" max="29" customWidth="true" width="22.7109375"/>
+    <col min="30" max="30" customWidth="true" width="21.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="22" customFormat="1" x14ac:dyDescent="0.25">
@@ -2801,22 +2802,22 @@
       <c r="AD20" s="8"/>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="D21"/>
+      <c r="D21" s="18"/>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="D22"/>
+      <c r="D22" s="18"/>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="D23"/>
+      <c r="D23" s="18"/>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="D24"/>
+      <c r="D24" s="18"/>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="D25"/>
+      <c r="D25" s="18"/>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="D26"/>
+      <c r="D26" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -2846,9 +2847,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="15" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" style="15" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="15" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="15" width="14.42578125"/>
+    <col min="2" max="2" customWidth="true" style="15" width="27.28515625"/>
+    <col min="3" max="3" customWidth="true" style="15" width="17.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -3037,12 +3038,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="36.42578125" customWidth="1"/>
-    <col min="4" max="4" width="42.7109375" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="12" width="14.28515625"/>
+    <col min="2" max="2" customWidth="true" width="17.42578125"/>
+    <col min="3" max="3" customWidth="true" width="36.42578125"/>
+    <col min="4" max="4" customWidth="true" width="42.7109375"/>
+    <col min="5" max="5" customWidth="true" width="24.7109375"/>
+    <col min="6" max="6" customWidth="true" width="25.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
se modifico la plantilla de oferta cademica
</commit_message>
<xml_diff>
--- a/schedule-management-backend/src/main/resources/files/templates/Plantilla_oferta_academica.xlsx
+++ b/schedule-management-backend/src/main/resources/files/templates/Plantilla_oferta_academica.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNIVERSIDAD\OCTAVO SEMESTRE\Proyecto_1\project-1-folder\schedule-management-unicauca\schedule-management-backend\src\main\resources\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A981E7-3009-4610-A338-E34739A0DB3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715D6B38-4C8C-4552-8D2D-975F870DF74C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{BB4D6D1C-47BE-482B-8849-6E1103E0D03C}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
   <si>
     <t>INFORMACION DEL PROGRAMA</t>
   </si>
@@ -58,13 +58,7 @@
     <t>NOMBRE</t>
   </si>
   <si>
-    <t>Ingenieria de Sistemas</t>
-  </si>
-  <si>
     <t>CODIGO</t>
-  </si>
-  <si>
-    <t>PIS</t>
   </si>
   <si>
     <t>INFORMACION DEL PERIODO</t>
@@ -106,34 +100,19 @@
     <t>PROFESOR 3</t>
   </si>
   <si>
-    <t>Erwin Meza Vega</t>
-  </si>
-  <si>
     <t>CÓDIGO</t>
   </si>
   <si>
     <t>DEPARTAMENTO</t>
   </si>
   <si>
-    <t>ESTR2 - Estructuras 2</t>
-  </si>
-  <si>
     <t>INTENSIDAD DE BLOQUE</t>
-  </si>
-  <si>
-    <t>POO - Cálculo 1</t>
   </si>
   <si>
     <t>SEMESTRE 1</t>
   </si>
   <si>
     <t>SEMESTRE 2</t>
-  </si>
-  <si>
-    <t>SI</t>
-  </si>
-  <si>
-    <t>INTRO1-Introducción a la programación</t>
   </si>
   <si>
     <t>SEMESTRE 3</t>
@@ -163,16 +142,7 @@
     <t>LISTADO DE MATERIAS DE CADA UNO DE LOS SEMESTRES</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>TIPO(S) DE AMBIENTE(S) REQUERIDO(S)</t>
-  </si>
-  <si>
-    <t>Salon y Laboratorio</t>
-  </si>
-  <si>
-    <t>2023-1</t>
   </si>
   <si>
     <t>EN BLOQUE</t>
@@ -410,6 +380,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -439,9 +412,6 @@
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -760,7 +730,7 @@
   <dimension ref="A1:J100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,144 +748,114 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="16"/>
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="16"/>
+      <c r="B4" s="17"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>40</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B5" s="15"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="3">
-        <v>45056</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="5">
-        <v>45057</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="B7" s="5"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H9" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="19"/>
+      <c r="H9" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="19"/>
+      <c r="J9" s="20"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="E10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="6" t="s">
+      <c r="F10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="G10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="I10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H10" s="6" t="s">
+      <c r="J10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
-        <v>1</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>36</v>
-      </c>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
       <c r="C11" s="7" t="str">
         <f>IFERROR(VLOOKUP(B11,MATERIAS!$A$4:$C$80,2,FALSE),IFERROR(VLOOKUP(B11,MATERIAS!$D$4:$F$80,2,FALSE),IFERROR(VLOOKUP(B11,MATERIAS!$G$4:$I$80,2,FALSE),IFERROR(VLOOKUP(B11,MATERIAS!$J$4:$L$80,2,FALSE),IFERROR(VLOOKUP(B11,MATERIAS!$M$4:$O$80,2,FALSE),IFERROR(VLOOKUP(B11,MATERIAS!$P$4:$R$80,2,FALSE),IFERROR(VLOOKUP(B11,MATERIAS!$S$4:$U$80,2,FALSE),IFERROR(VLOOKUP(B11,MATERIAS!$V$4:$X$80,2,FALSE),IFERROR(VLOOKUP(B11,MATERIAS!$Y$4:$AA$80,2,FALSE),IFERROR(VLOOKUP(B11,MATERIAS!$F$4:$AD$80,2,FALSE),"Sin programar"))))))))))</f>
-        <v>SI</v>
+        <v>Sin programar</v>
       </c>
       <c r="D11" s="14">
         <f>IFERROR(VLOOKUP(B11,MATERIAS!$A$4:$C$80,3,FALSE),IFERROR(VLOOKUP(B11,MATERIAS!$D$4:$F$80,3,FALSE),IFERROR(VLOOKUP(B11,MATERIAS!$G$4:$I$80,3,FALSE),IFERROR(VLOOKUP(B11,MATERIAS!$J$4:$L$80,3,FALSE),IFERROR(VLOOKUP(B11,MATERIAS!$M$4:$O$80,3,FALSE),IFERROR(VLOOKUP(B11,MATERIAS!$P$4:$R$80,3,FALSE),IFERROR(VLOOKUP(B11,MATERIAS!$S$4:$U$80,3,FALSE),IFERROR(VLOOKUP(B11,MATERIAS!$V$4:$X$80,3,FALSE),IFERROR(VLOOKUP(B11,MATERIAS!$Y$4:$AA$80,3,FALSE),IFERROR(VLOOKUP(B11,MATERIAS!$F$4:$AD$80,3,FALSE),0))))))))))</f>
-        <v>4</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="7">
-        <v>25</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>18</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
-        <v>2</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>23</v>
-      </c>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
       <c r="C12" s="7" t="str">
         <f>IFERROR(VLOOKUP(B12,MATERIAS!$A$4:$C$80,2,FALSE),IFERROR(VLOOKUP(B12,MATERIAS!$D$4:$F$80,2,FALSE),IFERROR(VLOOKUP(B12,MATERIAS!$G$4:$I$80,2,FALSE),IFERROR(VLOOKUP(B12,MATERIAS!$J$4:$L$80,2,FALSE),IFERROR(VLOOKUP(B12,MATERIAS!$M$4:$O$80,2,FALSE),IFERROR(VLOOKUP(B12,MATERIAS!$P$4:$R$80,2,FALSE),IFERROR(VLOOKUP(B12,MATERIAS!$S$4:$U$80,2,FALSE),IFERROR(VLOOKUP(B12,MATERIAS!$V$4:$X$80,2,FALSE),IFERROR(VLOOKUP(B12,MATERIAS!$Y$4:$AA$80,2,FALSE),IFERROR(VLOOKUP(B12,MATERIAS!$F$4:$AD$80,2,FALSE),"Sin programar"))))))))))</f>
-        <v>SI</v>
+        <v>Sin programar</v>
       </c>
       <c r="D12" s="14">
         <f>IFERROR(VLOOKUP(B12,MATERIAS!$A$4:$C$80,3,FALSE),IFERROR(VLOOKUP(B12,MATERIAS!$D$4:$F$80,3,FALSE),IFERROR(VLOOKUP(B12,MATERIAS!$G$4:$I$80,3,FALSE),IFERROR(VLOOKUP(B12,MATERIAS!$J$4:$L$80,3,FALSE),IFERROR(VLOOKUP(B12,MATERIAS!$M$4:$O$80,3,FALSE),IFERROR(VLOOKUP(B12,MATERIAS!$P$4:$R$80,3,FALSE),IFERROR(VLOOKUP(B12,MATERIAS!$S$4:$U$80,3,FALSE),IFERROR(VLOOKUP(B12,MATERIAS!$V$4:$X$80,3,FALSE),IFERROR(VLOOKUP(B12,MATERIAS!$Y$4:$AA$80,3,FALSE),IFERROR(VLOOKUP(B12,MATERIAS!$F$4:$AD$80,3,FALSE),0))))))))))</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -925,9 +865,7 @@
       <c r="J12" s="7"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
-        <v>2</v>
-      </c>
+      <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7" t="str">
         <f>IFERROR(VLOOKUP(B13,MATERIAS!$A$4:$C$80,2,FALSE),IFERROR(VLOOKUP(B13,MATERIAS!$D$4:$F$80,2,FALSE),IFERROR(VLOOKUP(B13,MATERIAS!$G$4:$I$80,2,FALSE),IFERROR(VLOOKUP(B13,MATERIAS!$J$4:$L$80,2,FALSE),IFERROR(VLOOKUP(B13,MATERIAS!$M$4:$O$80,2,FALSE),IFERROR(VLOOKUP(B13,MATERIAS!$P$4:$R$80,2,FALSE),IFERROR(VLOOKUP(B13,MATERIAS!$S$4:$U$80,2,FALSE),IFERROR(VLOOKUP(B13,MATERIAS!$V$4:$X$80,2,FALSE),IFERROR(VLOOKUP(B13,MATERIAS!$Y$4:$AA$80,2,FALSE),IFERROR(VLOOKUP(B13,MATERIAS!$F$4:$AD$80,2,FALSE),"Sin programar"))))))))))</f>
@@ -2559,7 +2497,7 @@
   <dimension ref="A1:AD80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2587,275 +2525,215 @@
     <col min="30" max="30" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="21"/>
-      <c r="AC1" s="21"/>
-      <c r="AD1" s="21"/>
+    <row r="1" spans="1:30" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="24"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="24"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="24"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="24"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="22" t="s">
+      <c r="Q2" s="24"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="22" t="s">
+      <c r="T2" s="24"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="W2" s="24"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z2" s="24"/>
+      <c r="AA2" s="25"/>
+      <c r="AB2" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="23"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" s="23"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" s="23"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="T2" s="23"/>
-      <c r="U2" s="24"/>
-      <c r="V2" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="W2" s="23"/>
-      <c r="X2" s="24"/>
-      <c r="Y2" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z2" s="23"/>
-      <c r="AA2" s="24"/>
-      <c r="AB2" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC2" s="23"/>
-      <c r="AD2" s="24"/>
+      <c r="AC2" s="24"/>
+      <c r="AD2" s="25"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="N3" s="11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Q3" s="11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="S3" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="T3" s="11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="V3" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="W3" s="11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="X3" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Y3" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Z3" s="11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="AA3" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AB3" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AC3" s="11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="AD3" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="7">
-        <v>4</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="7">
-        <v>4</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="7">
-        <v>4</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" s="7">
-        <v>4</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="N4" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="O4" s="7">
-        <v>4</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q4" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="R4" s="7">
-        <v>4</v>
-      </c>
-      <c r="S4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="T4" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="U4" s="7">
-        <v>4</v>
-      </c>
-      <c r="V4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="W4" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="X4" s="7">
-        <v>4</v>
-      </c>
-      <c r="Y4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z4" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA4" s="7">
-        <v>4</v>
-      </c>
-      <c r="AB4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC4" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD4" s="7">
-        <v>4</v>
-      </c>
+      <c r="A4" s="7"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="12"/>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="7"/>
+      <c r="AC4" s="12"/>
+      <c r="AD4" s="7"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
@@ -5324,13 +5202,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>